<commit_message>
Gestion de projet MPM Taches
</commit_message>
<xml_diff>
--- a/26. Recherche opérationnelle en Excel/09 - MULTIPLE - EXCELLENT FICHIER AVEC PRODUCTION,MELANGE,CUTSTOCK/02. Examples de programmes linéaires en Français.xlsx
+++ b/26. Recherche opérationnelle en Excel/09 - MULTIPLE - EXCELLENT FICHIER AVEC PRODUCTION,MELANGE,CUTSTOCK/02. Examples de programmes linéaires en Français.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\python-data-science\26. Recherche opérationnelle en Excel\09 - MULTIPLE - EXCELLENT FICHIER AVEC PRODUCTION,MELANGE,CUTSTOCK\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16320" windowHeight="5772" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16320" windowHeight="5772" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -4653,6 +4653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5408,6 +5409,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6418,9 +6420,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I15" sqref="I15:M15"/>
     </sheetView>
   </sheetViews>
@@ -7556,10 +7559,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.6"/>
@@ -9194,10 +9198,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.6"/>
@@ -9967,6 +9972,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -11176,6 +11182,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -12129,6 +12136,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>

</xml_diff>